<commit_message>
update excel data final
</commit_message>
<xml_diff>
--- a/students.xlsx
+++ b/students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>center</t>
   </si>
@@ -36,24 +36,12 @@
     <t>examName</t>
   </si>
   <si>
-    <t>talent search</t>
-  </si>
-  <si>
     <t>P.P SAVANI VIDHYAMANDIR KATHGADH</t>
   </si>
   <si>
     <t>01-Feb-2026</t>
   </si>
   <si>
-    <t>01-Feb-2027</t>
-  </si>
-  <si>
-    <t>01-Feb-2028</t>
-  </si>
-  <si>
-    <t>01-Feb-2029</t>
-  </si>
-  <si>
     <t>HARENDRASINH PARMAR</t>
   </si>
   <si>
@@ -76,6 +64,9 @@
   </si>
   <si>
     <t>GUJARATI</t>
+  </si>
+  <si>
+    <t>TALENT SEARCH EXAMINATION 2026</t>
   </si>
 </sst>
 </file>
@@ -418,8 +409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -427,7 +418,7 @@
     <col min="1" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="19.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="48.85546875" customWidth="1"/>
     <col min="7" max="7" width="53.28515625" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
   </cols>
@@ -437,10 +428,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -460,13 +451,13 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1">
         <v>9867775626</v>
@@ -475,24 +466,24 @@
         <v>88</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3">
         <v>10</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1">
         <v>9556526457</v>
@@ -501,24 +492,24 @@
         <v>89</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1">
         <v>7856625499</v>
@@ -527,24 +518,24 @@
         <v>90</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1">
         <v>8989567899</v>
@@ -553,13 +544,13 @@
         <v>91</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>